<commit_message>
Ignora i file nella cartella Results
</commit_message>
<xml_diff>
--- a/Data/Template.xlsx
+++ b/Data/Template.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3A5FF6-5B3F-4406-B199-16F9E1EEDE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E5E362-F964-404B-9D2E-B71A49A3B59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="763" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="763" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ATP" sheetId="1" r:id="rId1"/>
     <sheet name="CalibPosition" sheetId="2" r:id="rId2"/>
     <sheet name="Calibration" sheetId="15" r:id="rId3"/>
     <sheet name="CalibrationVerification" sheetId="16" r:id="rId4"/>
-    <sheet name="UniformityWhite" sheetId="17" r:id="rId5"/>
-    <sheet name="UniformityBlack" sheetId="19" r:id="rId6"/>
-    <sheet name="ChromaticityCoordinates" sheetId="8" r:id="rId7"/>
-    <sheet name="ContrastOnAxis" sheetId="7" r:id="rId8"/>
-    <sheet name="AnglesLuminance" sheetId="18" r:id="rId9"/>
+    <sheet name="FeedbackCalibration" sheetId="20" r:id="rId5"/>
+    <sheet name="UniformityWhite" sheetId="17" r:id="rId6"/>
+    <sheet name="UniformityBlack" sheetId="19" r:id="rId7"/>
+    <sheet name="ChromaticityCoordinates" sheetId="8" r:id="rId8"/>
+    <sheet name="ContrastOnAxis" sheetId="7" r:id="rId9"/>
+    <sheet name="AnglesLuminance" sheetId="18" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="ALGDAYRES">#REF!</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="199">
   <si>
     <t>Serial Number</t>
   </si>
@@ -649,6 +650,12 @@
   </si>
   <si>
     <t>DD-MM-YYYY</t>
+  </si>
+  <si>
+    <t>The TXT file is created in CalibratedCurve folder?</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -804,7 +811,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -896,12 +903,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1096,6 +1116,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1669,8 +1690,8 @@
   </sheetPr>
   <dimension ref="B1:N128"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1716,6 +1737,13 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="14" t="str">
+        <f>IF(D4="True","FAIL","PASS")</f>
+        <v>PASS</v>
+      </c>
       <c r="I4" s="25"/>
       <c r="L4" s="31" t="s">
         <v>194</v>
@@ -1728,6 +1756,9 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="14" t="b">
+        <v>1</v>
+      </c>
       <c r="I5"/>
       <c r="L5"/>
     </row>
@@ -3323,6 +3354,333 @@
   </sheetData>
   <pageMargins left="0.161811024" right="0.261811024" top="0.30118110199999998" bottom="0.143700787" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD79774-71DB-439E-B578-B428A438E377}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="B2:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="1.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.28515625" style="8"/>
+    <col min="2" max="2" width="25.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="1.28515625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="49">
+        <v>0</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="49">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="50" t="e">
+        <f>100*C5/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="50" t="e">
+        <f>IF(E5&gt;=75,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="49">
+        <v>2</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="50" t="e">
+        <f>100*C6/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="50" t="e">
+        <f>IF(E6&lt;=25,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="49">
+        <v>3</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="50" t="e">
+        <f>100*C7/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="50" t="e">
+        <f>IF(E7&gt;=80,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="49">
+        <v>4</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="50" t="e">
+        <f>100*C8/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="50" t="e">
+        <f>IF(E8&lt;=25,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="49">
+        <v>5</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="50" t="e">
+        <f>100*C9/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="50" t="e">
+        <f>IF(E9&lt;=20,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="49">
+        <v>6</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="50" t="e">
+        <f>100*C10/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" s="50" t="e">
+        <f>IF(E10&gt;=60,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="49">
+        <v>7</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="50" t="e">
+        <f>100*C11/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="50" t="e">
+        <f>IF(E11&gt;=75,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="49">
+        <v>8</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="50" t="e">
+        <f>100*C12/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="50" t="e">
+        <f>IF(E12&gt;=75,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="49">
+        <v>9</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="50" t="e">
+        <f>100*C13/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="50" t="e">
+        <f>IF(E13&gt;=60,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="49">
+        <v>10</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="50" t="e">
+        <f>100*C14/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="50" t="e">
+        <f>IF(E14&lt;=20,"PASS","FAIL")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="36"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="52"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="33"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="H23" s="54"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="36"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3572,8 +3930,8 @@
   </sheetPr>
   <dimension ref="B1:AA261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14015,6 +14373,39 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6B12A3-7638-41C5-A6D6-D6CB83D0247A}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="C4:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="80" t="str">
+        <f>IF(D4=TRUE,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1171DE-1924-4903-9906-E64D5CFE9BEA}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
@@ -14399,7 +14790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4C3780-50DF-466C-A213-DE9D13B3FCE9}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
@@ -14730,7 +15121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
@@ -14738,7 +15129,7 @@
   <dimension ref="B1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15421,7 +15812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
@@ -15429,7 +15820,7 @@
   <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15495,331 +15886,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD79774-71DB-439E-B578-B428A438E377}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="B2:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="1.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="1.28515625" style="8"/>
-    <col min="2" max="2" width="25.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="1.28515625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="49">
-        <v>0</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="37"/>
-    </row>
-    <row r="5" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="49">
-        <v>1</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="50" t="e">
-        <f>100*C5/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="50" t="e">
-        <f>IF(E5&gt;=75,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="49">
-        <v>2</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="50" t="e">
-        <f>100*C6/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="50" t="e">
-        <f>IF(E6&lt;=25,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="49">
-        <v>3</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" s="50" t="e">
-        <f>100*C7/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="50" t="e">
-        <f>IF(E7&gt;=80,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="49">
-        <v>4</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="50" t="e">
-        <f>100*C8/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="50" t="e">
-        <f>IF(E8&lt;=25,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" s="49">
-        <v>5</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="50" t="e">
-        <f>100*C9/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="50" t="e">
-        <f>IF(E9&lt;=20,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="49">
-        <v>6</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="50" t="e">
-        <f>100*C10/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="50" t="e">
-        <f>IF(E10&gt;=60,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="49">
-        <v>7</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="50" t="e">
-        <f>100*C11/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="50" t="e">
-        <f>IF(E11&gt;=75,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="49">
-        <v>8</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E12" s="50" t="e">
-        <f>100*C12/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="50" t="e">
-        <f>IF(E12&gt;=75,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="49">
-        <v>9</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="50" t="e">
-        <f>100*C13/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="50" t="e">
-        <f>IF(E13&gt;=60,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="49">
-        <v>10</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" s="50" t="e">
-        <f>100*C14/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="50" t="e">
-        <f>IF(E14&lt;=20,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="52"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="33"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="H23" s="54"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="36"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modifiche fatte dopo l'incontro del 30 ottobre 2025 con il Piazza
</commit_message>
<xml_diff>
--- a/Data/Template.xlsx
+++ b/Data/Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5B51A4-396D-4236-809C-7C91F69FBB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41784C74-0A08-4160-810A-B614AD009C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1531,8 +1531,8 @@
   </sheetPr>
   <dimension ref="B1:N128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2835,7 +2835,7 @@
   <dimension ref="B2:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3370,8 +3370,8 @@
   </sheetPr>
   <dimension ref="B1:AA261"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L265" sqref="L265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13752,15 +13752,13 @@
         <v>255</v>
       </c>
       <c r="K259" s="51">
-        <v>692.04707680042759</v>
+        <v>723.14</v>
       </c>
       <c r="L259" s="30">
-        <f>K259-K259*$U$1</f>
-        <v>622.84236912038477</v>
+        <v>685</v>
       </c>
       <c r="M259" s="30">
-        <f>K259+K259*$U$1</f>
-        <v>761.25178448047041</v>
+        <v>761.27</v>
       </c>
       <c r="N259" s="31"/>
       <c r="O259" s="28" t="str">
@@ -14569,7 +14567,7 @@
   <dimension ref="B1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I4" sqref="I4:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14678,37 +14676,16 @@
         <f t="shared" ref="H4:H6" si="0">IF(OR((F4=""),(G4="")),"",SQRT((F4-C4)^2+(G4-D4)^2))</f>
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="str">
-        <f>IF(H4="","",IF(H4&lt;E4,"PASS","FAIL"))</f>
-        <v>PASS</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="3" t="str">
-        <f>IF(ISBLANK($J$4),"",IF(J4&lt;1,(9.03*J4),(116*(POWER((J4/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L4" s="3" t="str">
-        <f>IF(OR(ISBLANK(DCHROMDEP),K4=""),"",13*K4*(F4-0.1978))</f>
-        <v/>
-      </c>
-      <c r="M4" s="3" t="str">
-        <f>IF(OR(ISBLANK(G4),K4=""),"",13*K4*(G4-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N4" s="3">
-        <f>IF(F4="","",F4-C4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <f>IF(G4="","",G4-D4)</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="10" t="e">
-        <f>IF(OR((N4=""),(O4="")),"",13*K4*SQRT((N4^2)+(O4^2)))</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="10"/>
       <c r="Q4" s="13" t="str">
-        <f>IF(H4="","N/A",IF(H4&gt;E4,"FAIL","PASS"))</f>
+        <f>IF(H4="","N/A",IF(H4&gt;=E4,"FAIL","PASS"))</f>
         <v>PASS</v>
       </c>
     </row>
@@ -14735,37 +14712,16 @@
         <f t="shared" si="0"/>
         <v>1.6360663189492046</v>
       </c>
-      <c r="I5" s="3" t="str">
-        <f>IF(H5="","",IF(H5&lt;E5,"PASS","FAIL"))</f>
-        <v>FAIL</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="3" t="str">
-        <f>IF(OR(ISBLANK($J$4),ISBLANK(J5)),"",IF(J5&lt;1,(9.03*J5),(116*(POWER((J5/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L5" s="3" t="str">
-        <f>IF(OR(ISBLANK(F5),K5=""),"",13*K5*(F5-0.1978))</f>
-        <v/>
-      </c>
-      <c r="M5" s="3" t="str">
-        <f>IF(OR(ISBLANK(G5),K5=""),"",13*K5*(G5-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N5" s="3">
-        <f t="shared" ref="N5:N6" si="1">IF(F5="","",F5-C5)</f>
-        <v>1.5680000000000001</v>
-      </c>
-      <c r="O5" s="3">
-        <f>IF(G5="","",G5-D5)</f>
-        <v>0.46699999999999997</v>
-      </c>
-      <c r="P5" s="10" t="e">
-        <f t="shared" ref="P5:P7" si="2">IF(OR((N5=""),(O5="")),"",13*K5*SQRT((N5^2)+(O5^2)))</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="10"/>
       <c r="Q5" s="13" t="str">
-        <f t="shared" ref="Q5:Q7" si="3">IF(H5="","N/A",IF(H5&gt;E5,"FAIL","PASS"))</f>
+        <f t="shared" ref="Q5:Q7" si="1">IF(H5="","N/A",IF(H5&gt;=E5,"FAIL","PASS"))</f>
         <v>FAIL</v>
       </c>
     </row>
@@ -14792,37 +14748,16 @@
         <f t="shared" si="0"/>
         <v>3.2199448753045448</v>
       </c>
-      <c r="I6" s="3" t="str">
-        <f t="shared" ref="I6" si="4">IF(H6="","",IF(H6&lt;E6,"PASS","FAIL"))</f>
-        <v>FAIL</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="3" t="str">
-        <f>IF(OR(ISBLANK($J$4),ISBLANK(J6)),"",IF(J6&lt;1,(9.03*J6),(116*(POWER((J6/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L6" s="3" t="str">
-        <f t="shared" ref="L6:L7" si="5">IF(OR(ISBLANK(F6),K6=""),"",13*K6*(F6-0.1978))</f>
-        <v/>
-      </c>
-      <c r="M6" s="3" t="str">
-        <f>IF(OR(ISBLANK(G6),K6=""),"",13*K6*(G6-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N6" s="3">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>2.883</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" ref="O6:O7" si="6">IF(G6="","",G6-D6)</f>
-        <v>1.4340000000000002</v>
-      </c>
-      <c r="P6" s="10" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q6" s="13" t="str">
-        <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -14849,37 +14784,16 @@
         <f>IF(OR((F7=""),(G7="")),"",SQRT((F7-C7)^2+(G7-D7)^2))</f>
         <v>4.7337063702768889</v>
       </c>
-      <c r="I7" s="3" t="str">
-        <f>IF(H7="","",IF(H7&lt;E7,"PASS","FAIL"))</f>
-        <v>FAIL</v>
-      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3" t="str">
-        <f>IF(OR(ISBLANK($J$4),ISBLANK(J7)),"",IF(J7&lt;1,(9.03*J7),(116*(POWER((J7/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L7" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="M7" s="3" t="str">
-        <f>IF(OR(ISBLANK(G7),K7=""),"",13*K7*(G7-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N7" s="3">
-        <f>IF(F7="","",F7-C7)</f>
-        <v>3.87</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="6"/>
-        <v>2.726</v>
-      </c>
-      <c r="P7" s="10" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="10"/>
       <c r="Q7" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -15031,37 +14945,16 @@
         <f>IF(OR((F20=""),(G20="")),"",SQRT((F20-C20)^2+(G20-D20)^2))</f>
         <v>0.9662235766115419</v>
       </c>
-      <c r="I20" s="3" t="str">
-        <f>IF(H20="","",IF(H20&lt;E20,"PASS","FAIL"))</f>
-        <v>FAIL</v>
-      </c>
+      <c r="I20" s="3"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="3" t="str">
-        <f>IF(ISBLANK($J$4),"",IF(J20&lt;1,(9.03*J20),(116*(POWER((J20/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L20" s="3" t="str">
-        <f>IF(OR(ISBLANK(DCHROMDEP),K20=""),"",13*K20*(F20-0.1978))</f>
-        <v/>
-      </c>
-      <c r="M20" s="3" t="str">
-        <f>IF(OR(ISBLANK(G20),K20=""),"",13*K20*(G20-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N20" s="3">
-        <f>IF(F20="","",F20-C20)</f>
-        <v>0.82800000000000007</v>
-      </c>
-      <c r="O20" s="3">
-        <f>IF(G20="","",G20-D20)</f>
-        <v>-0.498</v>
-      </c>
-      <c r="P20" s="10" t="e">
-        <f>IF(OR((N20=""),(O20="")),"",13*K20*SQRT((N20^2)+(O20^2)))</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="10"/>
       <c r="Q20" s="13" t="str">
-        <f>IF(H20="","N/A",IF(H20&gt;E20,"FAIL","PASS"))</f>
+        <f>IF(H20="","N/A",IF(H20&gt;=E20,"FAIL","PASS"))</f>
         <v>FAIL</v>
       </c>
     </row>
@@ -15088,37 +14981,16 @@
         <f>IF(OR((F21=""),(G21="")),"",SQRT((F21-C21)^2+(G21-D21)^2))</f>
         <v>1.6833543893072545</v>
       </c>
-      <c r="I21" s="3" t="str">
-        <f t="shared" ref="I21:I23" si="7">IF(H21="","",IF(H21&lt;E21,"PASS","FAIL"))</f>
-        <v>FAIL</v>
-      </c>
+      <c r="I21" s="3"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="3" t="str">
-        <f>IF(OR(ISBLANK($J$4),ISBLANK(J21)),"",IF(J21&lt;1,(9.03*J21),(116*(POWER((J21/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L21" s="3" t="str">
-        <f>IF(OR(ISBLANK(F21),K21=""),"",13*K21*(F21-0.1978))</f>
-        <v/>
-      </c>
-      <c r="M21" s="3" t="str">
-        <f>IF(OR(ISBLANK(G21),K21=""),"",13*K21*(G21-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N21" s="3">
-        <f t="shared" ref="N21:N23" si="8">IF(F21="","",F21-C21)</f>
-        <v>1.619</v>
-      </c>
-      <c r="O21" s="3">
-        <f>IF(G21="","",G21-D21)</f>
-        <v>0.46099999999999997</v>
-      </c>
-      <c r="P21" s="10" t="e">
-        <f t="shared" ref="P21:P23" si="9">IF(OR((N21=""),(O21="")),"",13*K21*SQRT((N21^2)+(O21^2)))</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="10"/>
       <c r="Q21" s="13" t="str">
-        <f t="shared" ref="Q21:Q23" si="10">IF(H21="","N/A",IF(H21&gt;E21,"FAIL","PASS"))</f>
+        <f t="shared" ref="Q21:Q23" si="2">IF(H21="","N/A",IF(H21&gt;=E21,"FAIL","PASS"))</f>
         <v>FAIL</v>
       </c>
     </row>
@@ -15142,40 +15014,19 @@
         <v>2</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" ref="H22:H23" si="11">IF(OR((F22=""),(G22="")),"",SQRT((F22-C22)^2+(G22-D22)^2))</f>
+        <f t="shared" ref="H22:H23" si="3">IF(OR((F22=""),(G22="")),"",SQRT((F22-C22)^2+(G22-D22)^2))</f>
         <v>3.2065245983775021</v>
       </c>
-      <c r="I22" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>FAIL</v>
-      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="3" t="str">
-        <f>IF(OR(ISBLANK($J$4),ISBLANK(J22)),"",IF(J22&lt;1,(9.03*J22),(116*(POWER((J22/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L22" s="3" t="str">
-        <f t="shared" ref="L22:L23" si="12">IF(OR(ISBLANK(F22),K22=""),"",13*K22*(F22-0.1978))</f>
-        <v/>
-      </c>
-      <c r="M22" s="3" t="str">
-        <f>IF(OR(ISBLANK(G22),K22=""),"",13*K22*(G22-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N22" s="3">
-        <f t="shared" si="8"/>
-        <v>2.87</v>
-      </c>
-      <c r="O22" s="3">
-        <f t="shared" ref="O22:O23" si="13">IF(G22="","",G22-D22)</f>
-        <v>1.4300000000000002</v>
-      </c>
-      <c r="P22" s="10" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="10"/>
       <c r="Q22" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -15199,40 +15050,19 @@
         <v>3</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>4.7406280174677287</v>
       </c>
-      <c r="I23" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>FAIL</v>
-      </c>
+      <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="3" t="str">
-        <f>IF(OR(ISBLANK($J$4),ISBLANK(J23)),"",IF(J23&lt;1,(9.03*J23),(116*(POWER((J23/$J$4),(1/3)))-16)))</f>
-        <v/>
-      </c>
-      <c r="L23" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="M23" s="3" t="str">
-        <f>IF(OR(ISBLANK(G23),K23=""),"",13*K23*(G23-0.4684))</f>
-        <v/>
-      </c>
-      <c r="N23" s="3">
-        <f t="shared" si="8"/>
-        <v>3.8450000000000002</v>
-      </c>
-      <c r="O23" s="3">
-        <f t="shared" si="13"/>
-        <v>2.7730000000000001</v>
-      </c>
-      <c r="P23" s="10" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="10"/>
       <c r="Q23" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -15260,7 +15090,7 @@
   <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sequenza di produzione ufficiale
</commit_message>
<xml_diff>
--- a/Data/Template.xlsx
+++ b/Data/Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41784C74-0A08-4160-810A-B614AD009C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96697630-DC53-40AD-AD47-5428B5387353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="155">
   <si>
     <t>Serial Number</t>
   </si>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>The TXT file is created in CalibratedCurve folder?</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -1531,8 +1534,8 @@
   </sheetPr>
   <dimension ref="B1:N128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1614,9 +1617,9 @@
       <c r="F7" s="20">
         <v>30</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="63" t="str">
         <f>UniformityWhite!B15</f>
-        <v>70</v>
+        <v>N/A</v>
       </c>
       <c r="I7" s="67" t="str">
         <f>IF(H7&gt;F7,"FAIL","PASS")</f>
@@ -1634,13 +1637,13 @@
       <c r="F8" s="20">
         <v>30</v>
       </c>
-      <c r="H8" s="63">
+      <c r="H8" s="63" t="str">
         <f>UniformityBlack!B15</f>
-        <v>7.6603135662882876E-2</v>
+        <v>N/A</v>
       </c>
       <c r="I8" s="67" t="str">
         <f>IF(H8&gt;F8,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="L8"/>
     </row>
@@ -1670,13 +1673,13 @@
       <c r="F11" s="20">
         <v>30</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="63" t="str">
         <f>UniformityWhite!I15</f>
-        <v>7.8166732090319685E-2</v>
+        <v>N/A</v>
       </c>
       <c r="I11" s="67" t="str">
         <f>IF(H11&gt;F11,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="L11"/>
     </row>
@@ -1690,13 +1693,13 @@
       <c r="F12" s="20">
         <v>30</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="63" t="str">
         <f>UniformityBlack!I15</f>
-        <v>7.8166732090319685E-2</v>
+        <v>N/A</v>
       </c>
       <c r="I12" s="67" t="str">
         <f>IF(H12&gt;F12,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="L12"/>
     </row>
@@ -2274,13 +2277,13 @@
       <c r="F47" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H47" s="66">
+      <c r="H47" s="66" t="e">
         <f>ChromaticityCoordinates!H4</f>
-        <v>0</v>
-      </c>
-      <c r="I47" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I47" s="69" t="e">
         <f>ChromaticityCoordinates!Q4</f>
-        <v>PASS</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="48" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,13 +2301,13 @@
       <c r="F48" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H48" s="66">
+      <c r="H48" s="66" t="e">
         <f>ChromaticityCoordinates!H5</f>
-        <v>1.6360663189492046</v>
-      </c>
-      <c r="I48" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I48" s="69" t="e">
         <f>ChromaticityCoordinates!Q5</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,13 +2325,13 @@
       <c r="F49" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H49" s="66">
+      <c r="H49" s="66" t="e">
         <f>ChromaticityCoordinates!H6</f>
-        <v>3.2199448753045448</v>
-      </c>
-      <c r="I49" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I49" s="69" t="e">
         <f>ChromaticityCoordinates!Q6</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2346,13 +2349,13 @@
       <c r="F50" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H50" s="66">
+      <c r="H50" s="66" t="e">
         <f>ChromaticityCoordinates!H7</f>
-        <v>4.7337063702768889</v>
-      </c>
-      <c r="I50" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I50" s="69" t="e">
         <f>ChromaticityCoordinates!Q7</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2390,13 +2393,13 @@
       <c r="F53" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H53" s="66">
+      <c r="H53" s="66" t="e">
         <f>ChromaticityCoordinates!H20</f>
-        <v>0.9662235766115419</v>
-      </c>
-      <c r="I53" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I53" s="69" t="e">
         <f>ChromaticityCoordinates!Q20</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="54" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2414,13 +2417,13 @@
       <c r="F54" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H54" s="66">
+      <c r="H54" s="66" t="e">
         <f>ChromaticityCoordinates!H21</f>
-        <v>1.6833543893072545</v>
-      </c>
-      <c r="I54" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I54" s="69" t="e">
         <f>ChromaticityCoordinates!Q21</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2438,13 +2441,13 @@
       <c r="F55" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H55" s="66">
+      <c r="H55" s="66" t="e">
         <f>ChromaticityCoordinates!H22</f>
-        <v>3.2065245983775021</v>
-      </c>
-      <c r="I55" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I55" s="69" t="e">
         <f>ChromaticityCoordinates!Q22</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="56" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,13 +2465,13 @@
       <c r="F56" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H56" s="66">
+      <c r="H56" s="66" t="e">
         <f>ChromaticityCoordinates!H23</f>
-        <v>4.7406280174677287</v>
-      </c>
-      <c r="I56" s="69" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I56" s="69" t="e">
         <f>ChromaticityCoordinates!Q23</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="57" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2491,13 +2494,13 @@
         <f>ContrastOnAxis!B3</f>
         <v>500</v>
       </c>
-      <c r="H59" s="66">
+      <c r="H59" s="66" t="e">
         <f>ContrastOnAxis!D3</f>
-        <v>182.79411506039997</v>
-      </c>
-      <c r="I59" s="67" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I59" s="67" t="e">
         <f>IF(H59&lt;=F59,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L59"/>
     </row>
@@ -2523,13 +2526,13 @@
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
-      <c r="H62" s="66">
-        <f>AnglesLuminance!C5</f>
-        <v>1</v>
-      </c>
-      <c r="I62" s="67" t="str">
+      <c r="H62" s="66" t="e">
+        <f>AnglesLuminance!E5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I62" s="67" t="e">
         <f>IF(H62&lt;=D62,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L62"/>
     </row>
@@ -2542,13 +2545,13 @@
       <c r="F63" s="20">
         <v>25</v>
       </c>
-      <c r="H63" s="66">
-        <f>AnglesLuminance!C6</f>
-        <v>2</v>
-      </c>
-      <c r="I63" s="67" t="str">
+      <c r="H63" s="66" t="e">
+        <f>AnglesLuminance!E6</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I63" s="67" t="e">
         <f>IF(H63&gt;=F63,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L63"/>
     </row>
@@ -2561,13 +2564,13 @@
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="20"/>
-      <c r="H64" s="66">
-        <f>AnglesLuminance!C7</f>
-        <v>3</v>
-      </c>
-      <c r="I64" s="67" t="str">
+      <c r="H64" s="66" t="e">
+        <f>AnglesLuminance!E7</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I64" s="67" t="e">
         <f>IF(H64&lt;=D64,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L64"/>
     </row>
@@ -2580,13 +2583,13 @@
       <c r="F65" s="20">
         <v>25</v>
       </c>
-      <c r="H65" s="66">
-        <f>AnglesLuminance!C8</f>
-        <v>4</v>
-      </c>
-      <c r="I65" s="67" t="str">
+      <c r="H65" s="66" t="e">
+        <f>AnglesLuminance!E8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I65" s="67" t="e">
         <f>IF(H65&gt;=F65,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L65"/>
     </row>
@@ -2599,13 +2602,13 @@
       <c r="F66" s="20">
         <v>20</v>
       </c>
-      <c r="H66" s="66">
-        <f>AnglesLuminance!C9</f>
-        <v>5</v>
-      </c>
-      <c r="I66" s="67" t="str">
+      <c r="H66" s="66" t="e">
+        <f>AnglesLuminance!E9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I66" s="67" t="e">
         <f>IF(H66&gt;=F66,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L66"/>
     </row>
@@ -2618,13 +2621,13 @@
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
-      <c r="H67" s="66">
-        <f>AnglesLuminance!C10</f>
-        <v>6</v>
-      </c>
-      <c r="I67" s="67" t="str">
+      <c r="H67" s="66" t="e">
+        <f>AnglesLuminance!E10</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I67" s="67" t="e">
         <f>IF(H67&lt;=D67,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L67"/>
     </row>
@@ -2637,13 +2640,13 @@
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="20"/>
-      <c r="H68" s="66">
-        <f>AnglesLuminance!C11</f>
-        <v>7</v>
-      </c>
-      <c r="I68" s="67" t="str">
+      <c r="H68" s="66" t="e">
+        <f>AnglesLuminance!E11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I68" s="67" t="e">
         <f>IF(H68&lt;=D68,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L68"/>
     </row>
@@ -2656,13 +2659,13 @@
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
-      <c r="H69" s="66">
-        <f>AnglesLuminance!C12</f>
-        <v>8</v>
-      </c>
-      <c r="I69" s="67" t="str">
+      <c r="H69" s="66" t="e">
+        <f>AnglesLuminance!E12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I69" s="67" t="e">
         <f>IF(H69&lt;=D69,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L69"/>
     </row>
@@ -2675,13 +2678,13 @@
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
-      <c r="H70" s="66">
-        <f>AnglesLuminance!C13</f>
-        <v>9</v>
-      </c>
-      <c r="I70" s="67" t="str">
+      <c r="H70" s="66" t="e">
+        <f>AnglesLuminance!E13</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I70" s="67" t="e">
         <f>IF(H70&lt;=D70,"FAIL","PASS")</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L70"/>
     </row>
@@ -2694,13 +2697,13 @@
       <c r="F71" s="20">
         <v>20</v>
       </c>
-      <c r="H71" s="66">
-        <f>AnglesLuminance!C14</f>
-        <v>10</v>
-      </c>
-      <c r="I71" s="67" t="str">
+      <c r="H71" s="66" t="e">
+        <f>AnglesLuminance!E14</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I71" s="67" t="e">
         <f>IF(H71&gt;=F71,"FAIL","PASS")</f>
-        <v>PASS</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L71"/>
     </row>
@@ -2835,7 +2838,7 @@
   <dimension ref="B2:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2876,7 +2879,7 @@
         <v>70</v>
       </c>
       <c r="C4" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>71</v>
@@ -2890,190 +2893,190 @@
       <c r="B5" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="40">
-        <v>1</v>
+      <c r="C5" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="41" t="e">
         <f>100*C5/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F5" s="41" t="e">
         <f>IF(E5&gt;=75,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="40">
-        <v>2</v>
+      <c r="C6" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>75</v>
       </c>
       <c r="E6" s="41" t="e">
         <f>100*C6/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F6" s="41" t="e">
         <f>IF(E6&lt;=25,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="40">
-        <v>3</v>
+      <c r="C7" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>77</v>
       </c>
       <c r="E7" s="41" t="e">
         <f>100*C7/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F7" s="41" t="e">
         <f>IF(E7&gt;=80,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="40">
-        <v>4</v>
+      <c r="C8" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>75</v>
       </c>
       <c r="E8" s="41" t="e">
         <f>100*C8/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F8" s="41" t="e">
         <f>IF(E8&lt;=25,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="40">
-        <v>5</v>
+      <c r="C9" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>80</v>
       </c>
       <c r="E9" s="41" t="e">
         <f>100*C9/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F9" s="41" t="e">
         <f>IF(E9&lt;=20,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="40">
-        <v>6</v>
+      <c r="C10" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="41" t="e">
         <f>100*C10/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F10" s="41" t="e">
         <f>IF(E10&gt;=60,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="40">
-        <v>7</v>
+      <c r="C11" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="41" t="e">
         <f>100*C11/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F11" s="41" t="e">
         <f>IF(E11&gt;=75,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="40">
-        <v>8</v>
+      <c r="C12" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="41" t="e">
         <f>100*C12/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F12" s="41" t="e">
         <f>IF(E12&gt;=75,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="40">
-        <v>9</v>
+      <c r="C13" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>82</v>
       </c>
       <c r="E13" s="41" t="e">
         <f>100*C13/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F13" s="41" t="e">
         <f>IF(E13&gt;=60,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="40">
-        <v>10</v>
+      <c r="C14" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="41" t="e">
         <f>100*C14/C4</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F14" s="41" t="e">
         <f>IF(E14&lt;=20,"PASS","FAIL")</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -3297,7 +3300,7 @@
   <dimension ref="B5:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,7 +3344,9 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>52311</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -3354,7 +3359,9 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>64335</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
   </sheetData>
@@ -3371,7 +3378,7 @@
   <dimension ref="B1:AA261"/>
   <sheetViews>
     <sheetView topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L265" sqref="L265"/>
+      <selection activeCell="O257" sqref="O257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13851,7 +13858,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14151,8 +14158,8 @@
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="50">
-        <v>70</v>
+      <c r="B15" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -14162,8 +14169,8 @@
       <c r="H15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="50">
-        <v>7.8166732090319685E-2</v>
+      <c r="I15" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
@@ -14236,7 +14243,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14535,8 +14542,8 @@
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="50">
-        <v>7.6603135662882876E-2</v>
+      <c r="B15" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -14546,8 +14553,8 @@
       <c r="H15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="50">
-        <v>7.8166732090319685E-2</v>
+      <c r="I15" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
@@ -14567,7 +14574,7 @@
   <dimension ref="B1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:P7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14666,15 +14673,15 @@
       <c r="E4" s="3">
         <v>0.03</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.184</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="F4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="3" t="e">
         <f t="shared" ref="H4:H6" si="0">IF(OR((F4=""),(G4="")),"",SQRT((F4-C4)^2+(G4-D4)^2))</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="4"/>
@@ -14684,9 +14691,9 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="10"/>
-      <c r="Q4" s="13" t="str">
+      <c r="Q4" s="13" t="e">
         <f>IF(H4="","N/A",IF(H4&gt;=E4,"FAIL","PASS"))</f>
-        <v>PASS</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14702,15 +14709,15 @@
       <c r="E5" s="3">
         <v>0.03</v>
       </c>
-      <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6360663189492046</v>
+      <c r="F5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="3" t="e">
+        <f>IF(OR((F5=""),(G5="")),"",SQRT((F5-C5)^2+(G5-D5)^2))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="4"/>
@@ -14720,9 +14727,9 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="13" t="str">
+      <c r="Q5" s="13" t="e">
         <f t="shared" ref="Q5:Q7" si="1">IF(H5="","N/A",IF(H5&gt;=E5,"FAIL","PASS"))</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14738,15 +14745,15 @@
       <c r="E6" s="3">
         <v>0.03</v>
       </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="F6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>3.2199448753045448</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="4"/>
@@ -14756,9 +14763,9 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="13" t="str">
+      <c r="Q6" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14774,15 +14781,15 @@
       <c r="E7" s="3">
         <v>0.03</v>
       </c>
-      <c r="F7" s="4">
-        <v>4</v>
-      </c>
-      <c r="G7" s="4">
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="F7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="3" t="e">
         <f>IF(OR((F7=""),(G7="")),"",SQRT((F7-C7)^2+(G7-D7)^2))</f>
-        <v>4.7337063702768889</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -14792,9 +14799,9 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="13" t="str">
+      <c r="Q7" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -14935,15 +14942,15 @@
       <c r="E20" s="3">
         <v>0.03</v>
       </c>
-      <c r="F20" s="4">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="F20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H20" s="3" t="e">
         <f>IF(OR((F20=""),(G20="")),"",SQRT((F20-C20)^2+(G20-D20)^2))</f>
-        <v>0.9662235766115419</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
@@ -14953,9 +14960,9 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="10"/>
-      <c r="Q20" s="13" t="str">
+      <c r="Q20" s="13" t="e">
         <f>IF(H20="","N/A",IF(H20&gt;=E20,"FAIL","PASS"))</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14971,15 +14978,15 @@
       <c r="E21" s="3">
         <v>0.03</v>
       </c>
-      <c r="F21" s="4">
-        <v>2</v>
-      </c>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="F21" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" s="3" t="e">
         <f>IF(OR((F21=""),(G21="")),"",SQRT((F21-C21)^2+(G21-D21)^2))</f>
-        <v>1.6833543893072545</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
@@ -14989,9 +14996,9 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="13" t="str">
+      <c r="Q21" s="13" t="e">
         <f t="shared" ref="Q21:Q23" si="2">IF(H21="","N/A",IF(H21&gt;=E21,"FAIL","PASS"))</f>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15007,15 +15014,15 @@
       <c r="E22" s="3">
         <v>0.03</v>
       </c>
-      <c r="F22" s="4">
-        <v>3</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="F22" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H22" s="3" t="e">
         <f t="shared" ref="H22:H23" si="3">IF(OR((F22=""),(G22="")),"",SQRT((F22-C22)^2+(G22-D22)^2))</f>
-        <v>3.2065245983775021</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
@@ -15025,9 +15032,9 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="10"/>
-      <c r="Q22" s="13" t="str">
+      <c r="Q22" s="13" t="e">
         <f t="shared" si="2"/>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15043,15 +15050,15 @@
       <c r="E23" s="3">
         <v>0.03</v>
       </c>
-      <c r="F23" s="4">
-        <v>4</v>
-      </c>
-      <c r="G23" s="4">
-        <v>3</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="F23" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="3" t="e">
         <f t="shared" si="3"/>
-        <v>4.7406280174677287</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -15061,9 +15068,9 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="13" t="str">
+      <c r="Q23" s="13" t="e">
         <f t="shared" si="2"/>
-        <v>FAIL</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -15090,7 +15097,7 @@
   <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15121,8 +15128,8 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1">
-        <v>182.79411506039997</v>
+      <c r="I2" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
@@ -15133,16 +15140,16 @@
         <v>500</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="e">
         <f>I2/I3</f>
-        <v>182.79411506039997</v>
-      </c>
-      <c r="E3" s="19" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E3" s="19" t="e">
         <f>IF(D3="","N/A",IF(OR(D3&lt;B3),"FAIL","PASS"))</f>
-        <v>FAIL</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>

</xml_diff>